<commit_message>
update utils from SVN
</commit_message>
<xml_diff>
--- a/utils/trunk/general/CMS Funding agencies.xlsx
+++ b/utils/trunk/general/CMS Funding agencies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="201">
   <si>
     <t>http://dx.doi.org/10.13039/501100002428</t>
   </si>
@@ -615,6 +615,18 @@
   </si>
   <si>
     <t>Universität Zürich</t>
+  </si>
+  <si>
+    <t>Welch Foundation</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.13039/100000928</t>
+  </si>
+  <si>
+    <t>Rachadapisek Sompot Fund for Postdoctoral Fellowship, Chulalongkorn University (Thailand)</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.13039/501100002873</t>
   </si>
 </sst>
 </file>
@@ -831,8 +843,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F93" totalsRowShown="0">
-  <autoFilter ref="A1:F93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F95" totalsRowShown="0">
+  <autoFilter ref="A1:F95"/>
   <tableColumns count="6">
     <tableColumn id="7" name="List order"/>
     <tableColumn id="1" name="Name"/>
@@ -1108,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D41" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2549,6 +2561,34 @@
         <v>139</v>
       </c>
       <c r="E93" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>199</v>
+      </c>
+      <c r="D94" t="s">
+        <v>200</v>
+      </c>
+      <c r="E94" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>18</v>
+      </c>
+      <c r="B95" t="s">
+        <v>197</v>
+      </c>
+      <c r="D95" t="s">
+        <v>198</v>
+      </c>
+      <c r="E95" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>